<commit_message>
Implemented extended "Guess Who?" game
</commit_message>
<xml_diff>
--- a/notes/Performance.xlsx
+++ b/notes/Performance.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340" xr2:uid="{7FAF82CF-59C1-4DE1-9728-4EB240A22499}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340" activeTab="1" xr2:uid="{7FAF82CF-59C1-4DE1-9728-4EB240A22499}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="original" sheetId="1" r:id="rId1"/>
+    <sheet name="extended" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Epochs</t>
   </si>
@@ -42,7 +43,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,53 +398,194 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7E14E3-454F-4468-8E08-B509556E5DAB}">
   <dimension ref="A1:L4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.453125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1">
+        <f>AVERAGE(B2:K2)</f>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.3082628225079293E-3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.9095577553190792E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.4710908785492296E-3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.8530175808177294E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.2638222665806999E-3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9.3769969908621496E-3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>9.2677511252798501E-3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>9.8293768810681394E-3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>9.4992075816135099E-3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9.3984958783356505E-3</v>
+      </c>
+      <c r="L3" s="1">
+        <f>AVERAGE(B3:K3)</f>
+        <v>9.5177579760933953E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1">
+        <v>100</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1">
+        <v>100</v>
+      </c>
+      <c r="K4" s="1">
+        <v>100</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4" si="0">AVERAGE(B4:K4)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CC624A-28D6-4FF1-B344-88B7BC86DC3E}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <v>24</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
         <v>28</v>
-      </c>
-      <c r="D2">
-        <v>27</v>
-      </c>
-      <c r="E2">
-        <v>24</v>
-      </c>
-      <c r="F2">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-      <c r="I2">
-        <v>30</v>
-      </c>
-      <c r="J2">
-        <v>27</v>
-      </c>
-      <c r="K2">
-        <v>23</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -443,46 +593,46 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.3082628225079293E-3</v>
+        <v>9.66444657890605E-3</v>
       </c>
       <c r="C3">
-        <v>9.9095577553190792E-3</v>
+        <v>9.4440245495377093E-3</v>
       </c>
       <c r="D3">
-        <v>9.4710908785492296E-3</v>
+        <v>9.5249566391610897E-3</v>
       </c>
       <c r="E3">
-        <v>9.8530175808177294E-3</v>
+        <v>8.8810657380027792E-3</v>
       </c>
       <c r="F3">
-        <v>9.2638222665806999E-3</v>
+        <v>8.9358881450378302E-3</v>
       </c>
       <c r="G3">
-        <v>9.3769969908621496E-3</v>
+        <v>9.3416104284196697E-3</v>
       </c>
       <c r="H3">
-        <v>9.2677511252798501E-3</v>
+        <v>9.6487291244979501E-3</v>
       </c>
       <c r="I3">
-        <v>9.8293768810681394E-3</v>
+        <v>9.4826913213637704E-3</v>
       </c>
       <c r="J3">
-        <v>9.4992075816135099E-3</v>
+        <v>9.5877916841543495E-3</v>
       </c>
       <c r="K3">
-        <v>9.3984958783356505E-3</v>
+        <v>9.4032569124210194E-3</v>
       </c>
       <c r="L3">
-        <f>AVERAGE(B3:K3)</f>
-        <v>9.5177579760933953E-3</v>
+        <f t="shared" ref="L3:L4" si="0">AVERAGE(B3:K3)</f>
+        <v>9.3914461121502226E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -516,7 +666,7 @@
         <v>100</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L3:L4" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generated part 3 jar
</commit_message>
<xml_diff>
--- a/notes/Performance.xlsx
+++ b/notes/Performance.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\St Andrews\Practicals\AI-Practice-A1\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\it41.home.cs.st-andrews.ac.uk\it41\workspace_win\CS5011-A1\AI-Practice-A1\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340" activeTab="1" xr2:uid="{7FAF82CF-59C1-4DE1-9728-4EB240A22499}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
     <sheet name="extended" sheetId="2" r:id="rId2"/>
+    <sheet name="resilient" sheetId="3" r:id="rId3"/>
+    <sheet name="manhattan" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>Epochs</t>
   </si>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,25 +397,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7E14E3-454F-4468-8E08-B509556E5DAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +454,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,7 +493,7 @@
         <v>9.5177579760933953E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,24 +538,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CC624A-28D6-4FF1-B344-88B7BC86DC3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +594,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -631,7 +633,7 @@
         <v>9.3914461121502226E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -668,6 +670,286 @@
       <c r="L4">
         <f t="shared" si="0"/>
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(B2:K2)</f>
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7.6553588721309501E-3</v>
+      </c>
+      <c r="C3">
+        <v>8.2030801441670097E-3</v>
+      </c>
+      <c r="D3">
+        <v>9.5119891508798002E-3</v>
+      </c>
+      <c r="E3">
+        <v>5.5308785975192298E-3</v>
+      </c>
+      <c r="F3">
+        <v>6.0333583969716196E-3</v>
+      </c>
+      <c r="G3">
+        <v>7.9914628855053804E-3</v>
+      </c>
+      <c r="H3">
+        <v>6.8242724506040802E-3</v>
+      </c>
+      <c r="I3">
+        <v>8.4940913522556193E-3</v>
+      </c>
+      <c r="J3">
+        <v>8.19632954536385E-3</v>
+      </c>
+      <c r="K3">
+        <v>9.8966589846971494E-3</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L4" si="0">AVERAGE(B3:K3)</f>
+        <v>7.8337480380094686E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>114</v>
+      </c>
+      <c r="C2">
+        <v>57</v>
+      </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>88</v>
+      </c>
+      <c r="G2">
+        <v>1229</v>
+      </c>
+      <c r="H2">
+        <v>54</v>
+      </c>
+      <c r="I2">
+        <v>51</v>
+      </c>
+      <c r="J2">
+        <v>33</v>
+      </c>
+      <c r="K2">
+        <v>34</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(B2:K2)</f>
+        <v>173.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>9.1875964263155498E-3</v>
+      </c>
+      <c r="C3">
+        <v>9.2501875913290101E-3</v>
+      </c>
+      <c r="D3">
+        <v>8.21787300942242E-3</v>
+      </c>
+      <c r="E3">
+        <v>3.2092278809168198E-3</v>
+      </c>
+      <c r="F3">
+        <v>7.5839334626915198E-3</v>
+      </c>
+      <c r="G3">
+        <v>9.9515606733849207E-3</v>
+      </c>
+      <c r="H3">
+        <v>9.0501865778718892E-3</v>
+      </c>
+      <c r="I3">
+        <v>9.1162618402570693E-3</v>
+      </c>
+      <c r="J3">
+        <v>8.9289267468090992E-3</v>
+      </c>
+      <c r="K3">
+        <v>8.0900947690678605E-3</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L4" si="0">AVERAGE(B3:K3)</f>
+        <v>8.2585848978066166E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>95.238095238095198</v>
+      </c>
+      <c r="C4">
+        <v>80.952380952380906</v>
+      </c>
+      <c r="D4">
+        <v>92.857142857142804</v>
+      </c>
+      <c r="E4">
+        <v>64.285714285714207</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>85.714285714285694</v>
+      </c>
+      <c r="H4">
+        <v>97.619047619047606</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>97.619047619047606</v>
+      </c>
+      <c r="K4">
+        <v>92.857142857142804</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>90.71428571428568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>